<commit_message>
Updating unit conversions for WebApp
</commit_message>
<xml_diff>
--- a/InputData/web-app/BpTPEU/BTU per Total Primary Energy Unit.xlsx
+++ b/InputData/web-app/BpTPEU/BTU per Total Primary Energy Unit.xlsx
@@ -1,27 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeRepositories\eps-us\InputData\web-app\BpTPEU\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mary Francis Swint\Vensim\eps-eu\InputData\web-app\BpTPEU\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18ACF8EC-DDAD-48C2-8393-9B9BDF10AC8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="390" windowWidth="27555" windowHeight="14100"/>
+    <workbookView xWindow="28680" yWindow="960" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="BpTPEU-large" sheetId="2" r:id="rId2"/>
     <sheet name="BpTPEU-small" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Source:</t>
   </si>
@@ -35,31 +49,37 @@
     <t>none needed</t>
   </si>
   <si>
-    <t>For the U.S.:</t>
-  </si>
-  <si>
     <t>large primary energy output unit</t>
   </si>
   <si>
     <t>small primary energy output unit</t>
   </si>
   <si>
-    <t>The large primary energy output unit (used in totals graphs) is: quadrillion BTU</t>
-  </si>
-  <si>
-    <t>The small primary energy output unit (used in energy intensity per unit GDP graphs) is: thousand BTU</t>
-  </si>
-  <si>
     <t>BpTPEU BTU per Large Primary Energy Unit</t>
   </si>
   <si>
     <t>BpTPEU BTU per Small Primary Energy Unit</t>
+  </si>
+  <si>
+    <t>For the EU.:</t>
+  </si>
+  <si>
+    <t>The large primary energy output unit (used in totals graphs) is: TWh</t>
+  </si>
+  <si>
+    <t>The small primary energy output unit (used in energy intensity per unit GDP graphs) is: MWh</t>
+  </si>
+  <si>
+    <t>Relevant Conversion Factors</t>
+  </si>
+  <si>
+    <t>BTU/MWh (pure unit conversion, not a heat rate)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -77,12 +97,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -97,14 +123,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -123,9 +150,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -163,9 +190,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -200,7 +227,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -235,7 +262,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -408,21 +435,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -443,17 +476,31 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="5"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>3412000</v>
+      </c>
+      <c r="B16" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -463,13 +510,56 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3">
+        <f>About!A16*10^6</f>
+        <v>3412000000000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="3"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr>
+    <tabColor theme="3"/>
+  </sheetPr>
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -485,48 +575,9 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3">
-        <f>10^15</f>
-        <v>1000000000000000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B9" s="3"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B10" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor theme="3"/>
-  </sheetPr>
-  <dimension ref="A1:B10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="4">
-        <f>10^3</f>
-        <v>1000</v>
+      <c r="B2">
+        <f>About!A16</f>
+        <v>3412000</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>